<commit_message>
error en creacion df performances para analisis estadistico - cambios añadidos en consecuencia
</commit_message>
<xml_diff>
--- a/Emmanuel/data/cleaned/modelos.xlsx
+++ b/Emmanuel/data/cleaned/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\Review_EDA_Emotion_Recognition\Emmanuel\data\cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5839ED-33AA-45E6-85D6-D3A395D83725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267D08AB-0DD4-4D30-B0D2-90953CA4D0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{64E64A21-F5DC-4B61-BBB1-A34825292E41}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="5">
   <si>
     <t>valence</t>
   </si>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9EA9D0-BE3F-477C-A7F5-6505C608D9A6}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>62.8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>58.7</v>
+        <v>52.04</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -442,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>56.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>56</v>
+        <v>54.05</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,127 +458,609 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>55.5</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>56.7</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>65.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>55.4</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>55</v>
+        <v>63.28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>54</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>53.5</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>62.8</v>
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>68.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>58.7</v>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>56.5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>56</v>
+        <v>72.08</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>55.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>56.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>59.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>55.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60.16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>53.5</v>
+        <v>65.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>58.52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>54.5</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>51.9</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>77.599999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>68.900000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>60.47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>55.92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1">
+        <v>52.04</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1">
+        <v>54.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="1">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1">
+        <v>63.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
+        <v>63.28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1">
+        <v>68.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>69.400000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1">
+        <v>72.08</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="1">
+        <v>59.71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="1">
+        <v>59.77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="1">
+        <v>60.16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="1">
+        <v>57.24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="1">
+        <v>65.63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="1">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="1">
+        <v>58.52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="1">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="1">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="1">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="1">
+        <v>77.599999999999994</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="1">
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="1">
+        <v>68.900000000000006</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="1">
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="1">
+        <v>60.47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="1">
+        <v>55.92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="1">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="1">
+        <v>27.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios generales producto de introduccion nuevas funciones
</commit_message>
<xml_diff>
--- a/Emmanuel/data/cleaned/modelos.xlsx
+++ b/Emmanuel/data/cleaned/modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\Review_EDA_Emotion_Recognition\Emmanuel\data\cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267D08AB-0DD4-4D30-B0D2-90953CA4D0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89079437-6940-488F-86BF-86F7379F1C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{64E64A21-F5DC-4B61-BBB1-A34825292E41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{64E64A21-F5DC-4B61-BBB1-A34825292E41}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="4">
   <si>
     <t>valence</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>performance</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
 </sst>
 </file>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9EA9D0-BE3F-477C-A7F5-6505C608D9A6}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:M31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,324 +741,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1">
-        <v>52.04</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1">
-        <v>54.05</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="1">
-        <v>64.400000000000006</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="1">
-        <v>65.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="1">
-        <v>63.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="1">
-        <v>63.28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>4</v>
-      </c>
-      <c r="B50" s="1">
-        <v>55.3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="1">
-        <v>64.400000000000006</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1">
-        <v>68.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="1">
-        <v>69.400000000000006</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="1">
-        <v>72.08</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1">
-        <v>59.71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="1">
-        <v>59.77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="1">
-        <v>60.16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="1">
-        <v>57.24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="1">
-        <v>65.63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="1">
-        <v>37.1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="1">
-        <v>69.8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="1">
-        <v>58.52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="1">
-        <v>54.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" s="1">
-        <v>51.9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" s="1">
-        <v>52.7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" s="1">
-        <v>50.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>4</v>
-      </c>
-      <c r="B70" s="1">
-        <v>53.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="1">
-        <v>77.599999999999994</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="1">
-        <v>82.2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="1">
-        <v>68.900000000000006</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="1">
-        <v>59.78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="1">
-        <v>60.47</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" s="1">
-        <v>55.92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="1">
-        <v>68.75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81" s="1">
-        <v>27.3</v>
-      </c>
+      <c r="B42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>